<commit_message>
WIP reviewed respawn times
Former-commit-id: cec2261f9c942f5d0d08e6522151f54788e550e0
</commit_message>
<xml_diff>
--- a/Docs/Progression/progression.xlsx
+++ b/Docs/Progression/progression.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22860" windowHeight="11640" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22860" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="12" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="395">
   <si>
     <t>SP_Archer01_Static</t>
   </si>
@@ -985,6 +986,228 @@
   </si>
   <si>
     <t>PF_MineMedium_Static</t>
+  </si>
+  <si>
+    <t>Falta añadir PF_Scaffold. Respawn time = 150</t>
+  </si>
+  <si>
+    <t>MineSmall</t>
+  </si>
+  <si>
+    <t>SP_MineSmall</t>
+  </si>
+  <si>
+    <t>PF_MineSmall</t>
+  </si>
+  <si>
+    <t>SP_MineSmall_Static</t>
+  </si>
+  <si>
+    <t>PF_MineSmall_Static</t>
+  </si>
+  <si>
+    <t>SP_OwlBig</t>
+  </si>
+  <si>
+    <t>PF_OwlBig</t>
+  </si>
+  <si>
+    <t>SP_OwlSmall</t>
+  </si>
+  <si>
+    <t>PF_OwlSmall</t>
+  </si>
+  <si>
+    <t>Piranha</t>
+  </si>
+  <si>
+    <t>SP_Piranha</t>
+  </si>
+  <si>
+    <t>PF_Piranha</t>
+  </si>
+  <si>
+    <t>PufferBird</t>
+  </si>
+  <si>
+    <t>SP_PufferBird</t>
+  </si>
+  <si>
+    <t>PF_PufferBird</t>
+  </si>
+  <si>
+    <t>Rat</t>
+  </si>
+  <si>
+    <t>SP_Rat</t>
+  </si>
+  <si>
+    <t>PF_Rat</t>
+  </si>
+  <si>
+    <t>SP_Richman</t>
+  </si>
+  <si>
+    <t>PF_Richman</t>
+  </si>
+  <si>
+    <t>SP_RichMan_Static</t>
+  </si>
+  <si>
+    <t>PF_RichMan_Static</t>
+  </si>
+  <si>
+    <t>Shark</t>
+  </si>
+  <si>
+    <t>SP_Shark</t>
+  </si>
+  <si>
+    <t>PF_Shark</t>
+  </si>
+  <si>
+    <t>SP_Sheep</t>
+  </si>
+  <si>
+    <t>PF_Sheep</t>
+  </si>
+  <si>
+    <t>SP_Sheep_Static</t>
+  </si>
+  <si>
+    <t>PF_Sheep_Static</t>
+  </si>
+  <si>
+    <t>ShieldMan</t>
+  </si>
+  <si>
+    <t>SP_Shieldman</t>
+  </si>
+  <si>
+    <t>PF_Shieldman</t>
+  </si>
+  <si>
+    <t>SP_Soldier01</t>
+  </si>
+  <si>
+    <t>PF_Soldier01</t>
+  </si>
+  <si>
+    <t>SP_Soldier01_Static</t>
+  </si>
+  <si>
+    <t>PF_Soldier01_Static</t>
+  </si>
+  <si>
+    <t>SP_Soldier02</t>
+  </si>
+  <si>
+    <t>PF_Soldier02</t>
+  </si>
+  <si>
+    <t>SP_Spartakus</t>
+  </si>
+  <si>
+    <t>PF_Spartakus</t>
+  </si>
+  <si>
+    <t>SpiderGreenTurret</t>
+  </si>
+  <si>
+    <t>SP_SpiderGreenTurret</t>
+  </si>
+  <si>
+    <t>PF_SpiderGreenTurret</t>
+  </si>
+  <si>
+    <t>SP_SpiderRed</t>
+  </si>
+  <si>
+    <t>PF_SpiderRed</t>
+  </si>
+  <si>
+    <t>SP_SpiderSmall</t>
+  </si>
+  <si>
+    <t>PF_SpiderSmall</t>
+  </si>
+  <si>
+    <t>SP_SpiderSmallTurret</t>
+  </si>
+  <si>
+    <t>PF_SpiderSmallTurret</t>
+  </si>
+  <si>
+    <t>SP_StarlingSmall_Flock</t>
+  </si>
+  <si>
+    <t>PF_Starling_Flock</t>
+  </si>
+  <si>
+    <t>SP_Starling_Flock</t>
+  </si>
+  <si>
+    <t>Troll</t>
+  </si>
+  <si>
+    <t>SP_Troll</t>
+  </si>
+  <si>
+    <t>PF_Troll</t>
+  </si>
+  <si>
+    <t>SP_TropicalFish</t>
+  </si>
+  <si>
+    <t>PF_TropicalFish</t>
+  </si>
+  <si>
+    <t>SP_Villager01</t>
+  </si>
+  <si>
+    <t>PF_Villager01</t>
+  </si>
+  <si>
+    <t>SP_Villager01_Static</t>
+  </si>
+  <si>
+    <t>PF_Villager01_Static</t>
+  </si>
+  <si>
+    <t>SP_Villager02</t>
+  </si>
+  <si>
+    <t>PF_Villager02</t>
+  </si>
+  <si>
+    <t>SP_Villager02_Static</t>
+  </si>
+  <si>
+    <t>PF_Villager02_Static</t>
+  </si>
+  <si>
+    <t>SP_witch</t>
+  </si>
+  <si>
+    <t>PF_Witch</t>
+  </si>
+  <si>
+    <t>SP_Worker01</t>
+  </si>
+  <si>
+    <t>PF_Worker01</t>
+  </si>
+  <si>
+    <t>SP_Worker02</t>
+  </si>
+  <si>
+    <t>PF_Worker02</t>
+  </si>
+  <si>
+    <t>SP_WorkerWife</t>
+  </si>
+  <si>
+    <t>PF_WorkerWife</t>
   </si>
 </sst>
 </file>
@@ -1535,27 +1758,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1804,11 +2007,11 @@
         </c:dLbls>
         <c:gapWidth val="228"/>
         <c:overlap val="100"/>
-        <c:axId val="96039680"/>
-        <c:axId val="96041216"/>
+        <c:axId val="64526976"/>
+        <c:axId val="64545152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="96039680"/>
+        <c:axId val="64526976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1818,7 +2021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96041216"/>
+        <c:crossAx val="64545152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1826,7 +2029,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96041216"/>
+        <c:axId val="64545152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1837,14 +2040,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96039680"/>
+        <c:crossAx val="64526976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2000,11 +2202,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102775040"/>
-        <c:axId val="107632512"/>
+        <c:axId val="65342848"/>
+        <c:axId val="65365504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102775040"/>
+        <c:axId val="65342848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2014,7 +2216,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107632512"/>
+        <c:crossAx val="65365504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2022,7 +2224,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107632512"/>
+        <c:axId val="65365504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2032,7 +2234,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102775040"/>
+        <c:crossAx val="65342848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2210,11 +2412,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="102438016"/>
-        <c:axId val="102439936"/>
+        <c:axId val="65385216"/>
+        <c:axId val="65387136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="102438016"/>
+        <c:axId val="65385216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2224,7 +2426,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102439936"/>
+        <c:crossAx val="65387136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2232,7 +2434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102439936"/>
+        <c:axId val="65387136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2242,7 +2444,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102438016"/>
+        <c:crossAx val="65385216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3222,8 +3424,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="D10:K64" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="D10:K64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="D10:K97" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="D10:K97"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Content Sku"/>
     <tableColumn id="2" name="Spawner Prefab"/>
@@ -3232,7 +3434,7 @@
     <tableColumn id="5" name="Respawn Max"/>
     <tableColumn id="6" name="HP Given"/>
     <tableColumn id="7" name="XP Given"/>
-    <tableColumn id="8" name="Damage" dataDxfId="4"/>
+    <tableColumn id="8" name="Damage" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3252,7 +3454,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="F8:K528" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table245" displayName="Table245" ref="F8:K528" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="F8:K528"/>
   <sortState ref="F9:M528">
     <sortCondition ref="F7:F527"/>
@@ -3263,7 +3465,7 @@
     <tableColumn id="5" name="respawn_time"/>
     <tableColumn id="6" name="activating_chance"/>
     <tableColumn id="7" name="XP"/>
-    <tableColumn id="8" name="total xp" dataDxfId="2">
+    <tableColumn id="8" name="total xp" dataDxfId="0">
       <calculatedColumnFormula>(Table245[[#This Row],[XP]]*Table245[[#This Row],[entity_spawned (AVG)]])*(Table245[[#This Row],[activating_chance]]/100)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3561,10 +3763,10 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="D5:K64"/>
+  <dimension ref="D5:K97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3584,6 +3786,11 @@
         <v>308</v>
       </c>
     </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>321</v>
+      </c>
+    </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
         <v>311</v>
@@ -3632,9 +3839,7 @@
       <c r="J11">
         <v>75</v>
       </c>
-      <c r="K11" s="73">
-        <v>10</v>
-      </c>
+      <c r="K11" s="73"/>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
@@ -3658,9 +3863,7 @@
       <c r="J12">
         <v>75</v>
       </c>
-      <c r="K12" s="73">
-        <v>10</v>
-      </c>
+      <c r="K12" s="73"/>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
@@ -3684,9 +3887,7 @@
       <c r="J13">
         <v>75</v>
       </c>
-      <c r="K13" s="73">
-        <v>15</v>
-      </c>
+      <c r="K13" s="73"/>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
@@ -3710,9 +3911,7 @@
       <c r="J14">
         <v>75</v>
       </c>
-      <c r="K14" s="73">
-        <v>15</v>
-      </c>
+      <c r="K14" s="73"/>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
@@ -3736,9 +3935,7 @@
       <c r="J15">
         <v>25</v>
       </c>
-      <c r="K15" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="K15" s="73"/>
     </row>
     <row r="16" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
@@ -3762,9 +3959,7 @@
       <c r="J16">
         <v>50</v>
       </c>
-      <c r="K16" s="73">
-        <v>3</v>
-      </c>
+      <c r="K16" s="73"/>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
@@ -3788,9 +3983,7 @@
       <c r="J17">
         <v>55</v>
       </c>
-      <c r="K17" s="73">
-        <v>8</v>
-      </c>
+      <c r="K17" s="73"/>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
@@ -3814,9 +4007,7 @@
       <c r="J18">
         <v>25</v>
       </c>
-      <c r="K18" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="K18" s="73"/>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
@@ -3840,9 +4031,7 @@
       <c r="J19">
         <v>25</v>
       </c>
-      <c r="K19" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="K19" s="73"/>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
@@ -3866,9 +4055,7 @@
       <c r="J20">
         <v>50</v>
       </c>
-      <c r="K20" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="K20" s="73"/>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
@@ -3892,9 +4079,7 @@
       <c r="J21">
         <v>50</v>
       </c>
-      <c r="K21" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="K21" s="73"/>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
@@ -3918,9 +4103,7 @@
       <c r="J22">
         <v>75</v>
       </c>
-      <c r="K22" s="73">
-        <v>8</v>
-      </c>
+      <c r="K22" s="73"/>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
@@ -3944,9 +4127,7 @@
       <c r="J23">
         <v>25</v>
       </c>
-      <c r="K23" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="K23" s="73"/>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
@@ -3970,9 +4151,7 @@
       <c r="J24">
         <v>25</v>
       </c>
-      <c r="K24" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="K24" s="73"/>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
@@ -3996,9 +4175,7 @@
       <c r="J25">
         <v>25</v>
       </c>
-      <c r="K25" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="K25" s="73"/>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
@@ -4022,9 +4199,7 @@
       <c r="J26">
         <v>25</v>
       </c>
-      <c r="K26" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="K26" s="73"/>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
@@ -4048,9 +4223,7 @@
       <c r="J27">
         <v>25</v>
       </c>
-      <c r="K27" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="K27" s="73"/>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
@@ -4074,9 +4247,7 @@
       <c r="J28">
         <v>25</v>
       </c>
-      <c r="K28" s="73" t="s">
-        <v>10</v>
-      </c>
+      <c r="K28" s="73"/>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
@@ -5007,6 +5178,864 @@
       </c>
       <c r="K64" s="73">
         <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>322</v>
+      </c>
+      <c r="E65" t="s">
+        <v>323</v>
+      </c>
+      <c r="F65" t="s">
+        <v>324</v>
+      </c>
+      <c r="G65">
+        <v>1500</v>
+      </c>
+      <c r="H65">
+        <v>1500</v>
+      </c>
+      <c r="I65">
+        <v>25</v>
+      </c>
+      <c r="J65">
+        <v>130</v>
+      </c>
+      <c r="K65" s="73">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>322</v>
+      </c>
+      <c r="E66" t="s">
+        <v>325</v>
+      </c>
+      <c r="F66" t="s">
+        <v>326</v>
+      </c>
+      <c r="G66">
+        <v>1500</v>
+      </c>
+      <c r="H66">
+        <v>1500</v>
+      </c>
+      <c r="I66">
+        <v>25</v>
+      </c>
+      <c r="J66">
+        <v>130</v>
+      </c>
+      <c r="K66" s="73">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>133</v>
+      </c>
+      <c r="E67" t="s">
+        <v>327</v>
+      </c>
+      <c r="F67" t="s">
+        <v>328</v>
+      </c>
+      <c r="G67">
+        <v>200</v>
+      </c>
+      <c r="H67">
+        <v>200</v>
+      </c>
+      <c r="I67">
+        <v>10</v>
+      </c>
+      <c r="J67">
+        <v>55</v>
+      </c>
+      <c r="K67" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>132</v>
+      </c>
+      <c r="E68" t="s">
+        <v>329</v>
+      </c>
+      <c r="F68" t="s">
+        <v>330</v>
+      </c>
+      <c r="G68">
+        <v>140</v>
+      </c>
+      <c r="H68">
+        <v>140</v>
+      </c>
+      <c r="I68">
+        <v>6</v>
+      </c>
+      <c r="J68">
+        <v>25</v>
+      </c>
+      <c r="K68" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>331</v>
+      </c>
+      <c r="E69" t="s">
+        <v>332</v>
+      </c>
+      <c r="F69" t="s">
+        <v>333</v>
+      </c>
+      <c r="G69">
+        <v>170</v>
+      </c>
+      <c r="H69">
+        <v>170</v>
+      </c>
+      <c r="I69">
+        <v>5</v>
+      </c>
+      <c r="J69">
+        <v>28</v>
+      </c>
+      <c r="K69" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>334</v>
+      </c>
+      <c r="E70" t="s">
+        <v>335</v>
+      </c>
+      <c r="F70" t="s">
+        <v>336</v>
+      </c>
+      <c r="G70">
+        <v>220</v>
+      </c>
+      <c r="H70">
+        <v>220</v>
+      </c>
+      <c r="I70">
+        <v>15</v>
+      </c>
+      <c r="J70">
+        <v>28</v>
+      </c>
+      <c r="K70" s="73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>337</v>
+      </c>
+      <c r="E71" t="s">
+        <v>338</v>
+      </c>
+      <c r="F71" t="s">
+        <v>339</v>
+      </c>
+      <c r="G71">
+        <v>120</v>
+      </c>
+      <c r="H71">
+        <v>120</v>
+      </c>
+      <c r="I71">
+        <v>2</v>
+      </c>
+      <c r="J71">
+        <v>25</v>
+      </c>
+      <c r="K71" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>87</v>
+      </c>
+      <c r="E72" t="s">
+        <v>340</v>
+      </c>
+      <c r="F72" t="s">
+        <v>341</v>
+      </c>
+      <c r="G72">
+        <v>260</v>
+      </c>
+      <c r="H72">
+        <v>260</v>
+      </c>
+      <c r="I72">
+        <v>15</v>
+      </c>
+      <c r="J72">
+        <v>75</v>
+      </c>
+      <c r="K72" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>87</v>
+      </c>
+      <c r="E73" t="s">
+        <v>342</v>
+      </c>
+      <c r="F73" t="s">
+        <v>343</v>
+      </c>
+      <c r="G73">
+        <v>260</v>
+      </c>
+      <c r="H73">
+        <v>260</v>
+      </c>
+      <c r="I73">
+        <v>15</v>
+      </c>
+      <c r="J73">
+        <v>75</v>
+      </c>
+      <c r="K73" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>344</v>
+      </c>
+      <c r="E74" t="s">
+        <v>345</v>
+      </c>
+      <c r="F74" t="s">
+        <v>346</v>
+      </c>
+      <c r="G74">
+        <v>350</v>
+      </c>
+      <c r="H74">
+        <v>350</v>
+      </c>
+      <c r="I74">
+        <v>30</v>
+      </c>
+      <c r="J74">
+        <v>83</v>
+      </c>
+      <c r="K74" s="73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>88</v>
+      </c>
+      <c r="E75" t="s">
+        <v>347</v>
+      </c>
+      <c r="F75" t="s">
+        <v>348</v>
+      </c>
+      <c r="G75">
+        <v>200</v>
+      </c>
+      <c r="H75">
+        <v>200</v>
+      </c>
+      <c r="I75">
+        <v>7</v>
+      </c>
+      <c r="J75">
+        <v>75</v>
+      </c>
+      <c r="K75" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>88</v>
+      </c>
+      <c r="E76" t="s">
+        <v>349</v>
+      </c>
+      <c r="F76" t="s">
+        <v>350</v>
+      </c>
+      <c r="G76">
+        <v>200</v>
+      </c>
+      <c r="H76">
+        <v>200</v>
+      </c>
+      <c r="I76">
+        <v>7</v>
+      </c>
+      <c r="J76">
+        <v>75</v>
+      </c>
+      <c r="K76" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>351</v>
+      </c>
+      <c r="E77" t="s">
+        <v>352</v>
+      </c>
+      <c r="F77" t="s">
+        <v>353</v>
+      </c>
+      <c r="G77">
+        <v>300</v>
+      </c>
+      <c r="H77">
+        <v>300</v>
+      </c>
+      <c r="I77">
+        <v>30</v>
+      </c>
+      <c r="J77">
+        <v>105</v>
+      </c>
+      <c r="K77" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>89</v>
+      </c>
+      <c r="E78" t="s">
+        <v>354</v>
+      </c>
+      <c r="F78" t="s">
+        <v>355</v>
+      </c>
+      <c r="G78">
+        <v>310</v>
+      </c>
+      <c r="H78">
+        <v>310</v>
+      </c>
+      <c r="I78">
+        <v>50</v>
+      </c>
+      <c r="J78">
+        <v>55</v>
+      </c>
+      <c r="K78" s="73">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="79" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>89</v>
+      </c>
+      <c r="E79" t="s">
+        <v>356</v>
+      </c>
+      <c r="F79" t="s">
+        <v>357</v>
+      </c>
+      <c r="G79">
+        <v>310</v>
+      </c>
+      <c r="H79">
+        <v>310</v>
+      </c>
+      <c r="I79">
+        <v>50</v>
+      </c>
+      <c r="J79">
+        <v>55</v>
+      </c>
+      <c r="K79" s="73">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="80" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>89</v>
+      </c>
+      <c r="E80" t="s">
+        <v>358</v>
+      </c>
+      <c r="F80" t="s">
+        <v>359</v>
+      </c>
+      <c r="G80">
+        <v>310</v>
+      </c>
+      <c r="H80">
+        <v>310</v>
+      </c>
+      <c r="I80">
+        <v>50</v>
+      </c>
+      <c r="J80">
+        <v>55</v>
+      </c>
+      <c r="K80" s="73">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>100</v>
+      </c>
+      <c r="E81" t="s">
+        <v>360</v>
+      </c>
+      <c r="F81" t="s">
+        <v>361</v>
+      </c>
+      <c r="G81">
+        <v>180</v>
+      </c>
+      <c r="H81">
+        <v>180</v>
+      </c>
+      <c r="I81">
+        <v>10</v>
+      </c>
+      <c r="J81">
+        <v>75</v>
+      </c>
+      <c r="K81" s="73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>362</v>
+      </c>
+      <c r="E82" t="s">
+        <v>363</v>
+      </c>
+      <c r="F82" t="s">
+        <v>364</v>
+      </c>
+      <c r="G82">
+        <v>170</v>
+      </c>
+      <c r="H82">
+        <v>170</v>
+      </c>
+      <c r="I82">
+        <v>20</v>
+      </c>
+      <c r="J82">
+        <v>55</v>
+      </c>
+      <c r="K82" s="73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>90</v>
+      </c>
+      <c r="E83" t="s">
+        <v>365</v>
+      </c>
+      <c r="F83" t="s">
+        <v>366</v>
+      </c>
+      <c r="G83">
+        <v>170</v>
+      </c>
+      <c r="H83">
+        <v>170</v>
+      </c>
+      <c r="I83">
+        <v>20</v>
+      </c>
+      <c r="J83">
+        <v>55</v>
+      </c>
+      <c r="K83" s="73">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>91</v>
+      </c>
+      <c r="E84" t="s">
+        <v>367</v>
+      </c>
+      <c r="F84" t="s">
+        <v>368</v>
+      </c>
+      <c r="G84">
+        <v>150</v>
+      </c>
+      <c r="H84">
+        <v>150</v>
+      </c>
+      <c r="I84">
+        <v>4</v>
+      </c>
+      <c r="J84">
+        <v>25</v>
+      </c>
+      <c r="K84" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>91</v>
+      </c>
+      <c r="E85" t="s">
+        <v>369</v>
+      </c>
+      <c r="F85" t="s">
+        <v>370</v>
+      </c>
+      <c r="G85">
+        <v>150</v>
+      </c>
+      <c r="H85">
+        <v>150</v>
+      </c>
+      <c r="I85">
+        <v>4</v>
+      </c>
+      <c r="J85">
+        <v>25</v>
+      </c>
+      <c r="K85" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>134</v>
+      </c>
+      <c r="E86" t="s">
+        <v>371</v>
+      </c>
+      <c r="F86" t="s">
+        <v>372</v>
+      </c>
+      <c r="G86">
+        <v>180</v>
+      </c>
+      <c r="H86">
+        <v>180</v>
+      </c>
+      <c r="I86">
+        <v>3</v>
+      </c>
+      <c r="J86">
+        <v>25</v>
+      </c>
+      <c r="K86" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>134</v>
+      </c>
+      <c r="E87" t="s">
+        <v>373</v>
+      </c>
+      <c r="F87" t="s">
+        <v>372</v>
+      </c>
+      <c r="G87">
+        <v>180</v>
+      </c>
+      <c r="H87">
+        <v>180</v>
+      </c>
+      <c r="I87">
+        <v>3</v>
+      </c>
+      <c r="J87">
+        <v>25</v>
+      </c>
+      <c r="K87" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>374</v>
+      </c>
+      <c r="E88" t="s">
+        <v>375</v>
+      </c>
+      <c r="F88" t="s">
+        <v>376</v>
+      </c>
+      <c r="G88">
+        <v>420</v>
+      </c>
+      <c r="H88">
+        <v>420</v>
+      </c>
+      <c r="I88">
+        <v>80</v>
+      </c>
+      <c r="J88">
+        <v>83</v>
+      </c>
+      <c r="K88" s="73">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>137</v>
+      </c>
+      <c r="E89" t="s">
+        <v>377</v>
+      </c>
+      <c r="F89" t="s">
+        <v>378</v>
+      </c>
+      <c r="G89">
+        <v>140</v>
+      </c>
+      <c r="H89">
+        <v>140</v>
+      </c>
+      <c r="I89">
+        <v>2</v>
+      </c>
+      <c r="J89">
+        <v>25</v>
+      </c>
+      <c r="K89" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>92</v>
+      </c>
+      <c r="E90" t="s">
+        <v>379</v>
+      </c>
+      <c r="F90" t="s">
+        <v>380</v>
+      </c>
+      <c r="G90">
+        <v>220</v>
+      </c>
+      <c r="H90">
+        <v>220</v>
+      </c>
+      <c r="I90">
+        <v>15</v>
+      </c>
+      <c r="J90">
+        <v>50</v>
+      </c>
+      <c r="K90" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>92</v>
+      </c>
+      <c r="E91" t="s">
+        <v>381</v>
+      </c>
+      <c r="F91" t="s">
+        <v>382</v>
+      </c>
+      <c r="G91">
+        <v>220</v>
+      </c>
+      <c r="H91">
+        <v>220</v>
+      </c>
+      <c r="I91">
+        <v>15</v>
+      </c>
+      <c r="J91">
+        <v>50</v>
+      </c>
+      <c r="K91" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>93</v>
+      </c>
+      <c r="E92" t="s">
+        <v>383</v>
+      </c>
+      <c r="F92" t="s">
+        <v>384</v>
+      </c>
+      <c r="G92">
+        <v>220</v>
+      </c>
+      <c r="H92">
+        <v>220</v>
+      </c>
+      <c r="I92">
+        <v>15</v>
+      </c>
+      <c r="J92">
+        <v>50</v>
+      </c>
+      <c r="K92" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>93</v>
+      </c>
+      <c r="E93" t="s">
+        <v>385</v>
+      </c>
+      <c r="F93" t="s">
+        <v>386</v>
+      </c>
+      <c r="G93">
+        <v>220</v>
+      </c>
+      <c r="H93">
+        <v>220</v>
+      </c>
+      <c r="I93">
+        <v>15</v>
+      </c>
+      <c r="J93">
+        <v>50</v>
+      </c>
+      <c r="K93" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>135</v>
+      </c>
+      <c r="E94" t="s">
+        <v>387</v>
+      </c>
+      <c r="F94" t="s">
+        <v>388</v>
+      </c>
+      <c r="G94">
+        <v>300</v>
+      </c>
+      <c r="H94">
+        <v>300</v>
+      </c>
+      <c r="I94">
+        <v>20</v>
+      </c>
+      <c r="J94">
+        <v>55</v>
+      </c>
+      <c r="K94" s="73">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>101</v>
+      </c>
+      <c r="E95" t="s">
+        <v>389</v>
+      </c>
+      <c r="F95" t="s">
+        <v>390</v>
+      </c>
+      <c r="G95">
+        <v>200</v>
+      </c>
+      <c r="H95">
+        <v>200</v>
+      </c>
+      <c r="I95">
+        <v>8</v>
+      </c>
+      <c r="J95">
+        <v>75</v>
+      </c>
+      <c r="K95" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>101</v>
+      </c>
+      <c r="E96" t="s">
+        <v>391</v>
+      </c>
+      <c r="F96" t="s">
+        <v>392</v>
+      </c>
+      <c r="G96">
+        <v>200</v>
+      </c>
+      <c r="H96">
+        <v>200</v>
+      </c>
+      <c r="I96">
+        <v>8</v>
+      </c>
+      <c r="J96">
+        <v>75</v>
+      </c>
+      <c r="K96" s="73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>101</v>
+      </c>
+      <c r="E97" t="s">
+        <v>393</v>
+      </c>
+      <c r="F97" t="s">
+        <v>394</v>
+      </c>
+      <c r="G97">
+        <v>200</v>
+      </c>
+      <c r="H97">
+        <v>200</v>
+      </c>
+      <c r="I97">
+        <v>8</v>
+      </c>
+      <c r="J97">
+        <v>75</v>
+      </c>
+      <c r="K97" s="73" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -9866,7 +10895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G2:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -21627,7 +22656,7 @@
         <v>20</v>
       </c>
       <c r="P6" s="51">
-        <f t="shared" ref="P6:P8" si="0">ROUND(O6/N6,2)</f>
+        <f>ROUND(O6/N6,2)</f>
         <v>0.4</v>
       </c>
       <c r="R6" s="61">
@@ -21654,7 +22683,7 @@
         <v>20</v>
       </c>
       <c r="P7" s="54">
-        <f t="shared" si="0"/>
+        <f>ROUND(O7/N7,2)</f>
         <v>0.33</v>
       </c>
       <c r="R7" s="61">
@@ -21681,7 +22710,7 @@
         <v>20</v>
       </c>
       <c r="P8" s="57">
-        <f t="shared" si="0"/>
+        <f>ROUND(O8/N8,2)</f>
         <v>0.28999999999999998</v>
       </c>
       <c r="R8" s="61">
@@ -21761,7 +22790,7 @@
         <v>35</v>
       </c>
       <c r="J13" s="48">
-        <f>$D$5</f>
+        <f t="shared" ref="J13:J24" si="0">$D$5</f>
         <v>20</v>
       </c>
       <c r="K13" s="48">
@@ -21780,11 +22809,11 @@
         <v>35</v>
       </c>
       <c r="J14" s="48">
-        <f t="shared" ref="J14:J17" si="1">$D$5</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="K14" s="48">
-        <f t="shared" ref="K14:K17" si="2">$I$41/$I$13</f>
+        <f>$I$41/$I$13</f>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -21796,11 +22825,11 @@
         <v>35</v>
       </c>
       <c r="J15" s="48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="K15" s="48">
-        <f t="shared" si="2"/>
+        <f>$I$41/$I$13</f>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -21812,11 +22841,11 @@
         <v>35</v>
       </c>
       <c r="J16" s="48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="K16" s="48">
-        <f t="shared" si="2"/>
+        <f>$I$41/$I$13</f>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -21828,11 +22857,11 @@
         <v>40</v>
       </c>
       <c r="J17" s="48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="K17" s="48">
-        <f t="shared" si="2"/>
+        <f>$I$41/$I$13</f>
         <v>2.5714285714285716</v>
       </c>
     </row>
@@ -21844,11 +22873,11 @@
         <v>50</v>
       </c>
       <c r="J18" s="51">
-        <f>$D$5</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="K18" s="51">
-        <f t="shared" ref="K18:K23" si="3">$I$41/$I$18</f>
+        <f t="shared" ref="K18:K23" si="1">$I$41/$I$18</f>
         <v>1.8</v>
       </c>
       <c r="L18" t="s">
@@ -21863,11 +22892,11 @@
         <v>50</v>
       </c>
       <c r="J19" s="51">
-        <f t="shared" ref="J19:J23" si="4">$D$5</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="K19" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
     </row>
@@ -21879,11 +22908,11 @@
         <v>50</v>
       </c>
       <c r="J20" s="51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="K20" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
     </row>
@@ -21895,11 +22924,11 @@
         <v>50</v>
       </c>
       <c r="J21" s="51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="K21" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
     </row>
@@ -21911,11 +22940,11 @@
         <v>50</v>
       </c>
       <c r="J22" s="51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="K22" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
     </row>
@@ -21927,11 +22956,11 @@
         <v>50</v>
       </c>
       <c r="J23" s="51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="K23" s="51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
     </row>
@@ -21943,7 +22972,7 @@
         <v>60</v>
       </c>
       <c r="J24" s="54">
-        <f>$D$5</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="K24" s="54">
@@ -21962,11 +22991,11 @@
         <v>60</v>
       </c>
       <c r="J25" s="54">
-        <f t="shared" ref="J25:J31" si="5">$D$5</f>
+        <f t="shared" ref="J25:J31" si="2">$D$5</f>
         <v>20</v>
       </c>
       <c r="K25" s="54">
-        <f t="shared" ref="K25:K31" si="6">$I$41/$I$24</f>
+        <f t="shared" ref="K25:K31" si="3">$I$41/$I$24</f>
         <v>1.5</v>
       </c>
     </row>
@@ -21978,11 +23007,11 @@
         <v>60</v>
       </c>
       <c r="J26" s="54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="K26" s="54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
     </row>
@@ -21994,11 +23023,11 @@
         <v>60</v>
       </c>
       <c r="J27" s="54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="K27" s="54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
     </row>
@@ -22010,11 +23039,11 @@
         <v>60</v>
       </c>
       <c r="J28" s="54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="K28" s="54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
     </row>
@@ -22026,11 +23055,11 @@
         <v>60</v>
       </c>
       <c r="J29" s="54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="K29" s="54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
     </row>
@@ -22042,11 +23071,11 @@
         <v>60</v>
       </c>
       <c r="J30" s="54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="K30" s="54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
     </row>
@@ -22058,11 +23087,11 @@
         <v>60</v>
       </c>
       <c r="J31" s="54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="K31" s="54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
     </row>
@@ -22093,11 +23122,11 @@
         <v>70</v>
       </c>
       <c r="J33" s="57">
-        <f t="shared" ref="J33:J40" si="7">$D$5</f>
+        <f t="shared" ref="J33:J40" si="4">$D$5</f>
         <v>20</v>
       </c>
       <c r="K33" s="57">
-        <f t="shared" ref="K33:K40" si="8">$I$41/$I$32</f>
+        <f t="shared" ref="K33:K40" si="5">$I$41/$I$32</f>
         <v>1.2857142857142858</v>
       </c>
     </row>
@@ -22109,11 +23138,11 @@
         <v>75</v>
       </c>
       <c r="J34" s="57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="K34" s="57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.2857142857142858</v>
       </c>
     </row>
@@ -22125,11 +23154,11 @@
         <v>75</v>
       </c>
       <c r="J35" s="57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="K35" s="57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.2857142857142858</v>
       </c>
     </row>
@@ -22141,11 +23170,11 @@
         <v>75</v>
       </c>
       <c r="J36" s="57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="K36" s="57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.2857142857142858</v>
       </c>
     </row>
@@ -22157,11 +23186,11 @@
         <v>80</v>
       </c>
       <c r="J37" s="57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="K37" s="57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.2857142857142858</v>
       </c>
     </row>
@@ -22173,11 +23202,11 @@
         <v>80</v>
       </c>
       <c r="J38" s="57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="K38" s="57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.2857142857142858</v>
       </c>
     </row>
@@ -22189,11 +23218,11 @@
         <v>80</v>
       </c>
       <c r="J39" s="57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="K39" s="57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.2857142857142858</v>
       </c>
     </row>
@@ -22205,11 +23234,11 @@
         <v>85</v>
       </c>
       <c r="J40" s="57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="K40" s="57">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.2857142857142858</v>
       </c>
     </row>
@@ -22236,7 +23265,7 @@
         <v>90</v>
       </c>
       <c r="J42" s="65">
-        <f t="shared" ref="J42:J51" si="9">$D$5</f>
+        <f t="shared" ref="J42:J51" si="6">$D$5</f>
         <v>20</v>
       </c>
       <c r="K42" s="65">
@@ -22251,7 +23280,7 @@
         <v>90</v>
       </c>
       <c r="J43" s="65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K43" s="65">
@@ -22266,7 +23295,7 @@
         <v>90</v>
       </c>
       <c r="J44" s="65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K44" s="65">
@@ -22281,7 +23310,7 @@
         <v>90</v>
       </c>
       <c r="J45" s="65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K45" s="65">
@@ -22296,7 +23325,7 @@
         <v>90</v>
       </c>
       <c r="J46" s="65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K46" s="65">
@@ -22311,7 +23340,7 @@
         <v>90</v>
       </c>
       <c r="J47" s="65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K47" s="65">
@@ -22326,7 +23355,7 @@
         <v>90</v>
       </c>
       <c r="J48" s="65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K48" s="65">
@@ -22341,7 +23370,7 @@
         <v>90</v>
       </c>
       <c r="J49" s="65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K49" s="65">
@@ -22356,7 +23385,7 @@
         <v>100</v>
       </c>
       <c r="J50" s="65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K50" s="65">
@@ -22371,7 +23400,7 @@
         <v>100</v>
       </c>
       <c r="J51" s="60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K51" s="60">

</xml_diff>

<commit_message>
WIP reviewing spawners stats. Added few background canaries/starlings
Former-commit-id: 050f5920132ac4950b593c2f7265fd4456bba9e0
</commit_message>
<xml_diff>
--- a/Docs/Progression/progression.xlsx
+++ b/Docs/Progression/progression.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22860" windowHeight="11640" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22860" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="12" r:id="rId1"/>
@@ -6943,8 +6943,8 @@
   </sheetPr>
   <dimension ref="B1:U270"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12442,8 +12442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P537"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Bug fixed in Troll attack
Former-commit-id: 7194b388b1c01dcd54c007e1e60f5da391fbedb4
</commit_message>
<xml_diff>
--- a/Docs/Progression/progression.xlsx
+++ b/Docs/Progression/progression.xlsx
@@ -17,7 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId7"/>
   </externalReferences>
-  <calcPr calcId="145621" calcMode="manual"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -2226,11 +2226,11 @@
         </c:dLbls>
         <c:gapWidth val="228"/>
         <c:overlap val="100"/>
-        <c:axId val="80863616"/>
-        <c:axId val="80865152"/>
+        <c:axId val="106588032"/>
+        <c:axId val="106589568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80863616"/>
+        <c:axId val="106588032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2240,7 +2240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80865152"/>
+        <c:crossAx val="106589568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2248,7 +2248,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80865152"/>
+        <c:axId val="106589568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2259,13 +2259,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80863616"/>
+        <c:crossAx val="106588032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2377,34 +2378,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>13.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>15.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>16.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>17.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>18.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>19.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>20.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2421,11 +2422,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83453056"/>
-        <c:axId val="83454976"/>
+        <c:axId val="67308160"/>
+        <c:axId val="67310336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83453056"/>
+        <c:axId val="67308160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2435,7 +2436,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83454976"/>
+        <c:crossAx val="67310336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2443,7 +2444,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83454976"/>
+        <c:axId val="67310336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2453,7 +2454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83453056"/>
+        <c:crossAx val="67308160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2587,34 +2588,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>16.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>22.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>21.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>27.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>27.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>30.3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>32.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>30.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>31.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>32.299999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2631,11 +2632,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83462400"/>
-        <c:axId val="83485056"/>
+        <c:axId val="67342336"/>
+        <c:axId val="67344256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83462400"/>
+        <c:axId val="67342336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2645,7 +2646,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83485056"/>
+        <c:crossAx val="67344256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2653,7 +2654,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83485056"/>
+        <c:axId val="67344256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2663,7 +2664,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83462400"/>
+        <c:crossAx val="67342336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2715,6 +2716,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2824,6 +2826,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2853,6 +2856,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2962,6 +2966,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2991,6 +2996,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3056,6 +3062,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3085,6 +3092,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3194,6 +3202,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3899,15 +3908,6 @@
           <cell r="Z16">
             <v>11</v>
           </cell>
-          <cell r="AV16">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-          <cell r="AW16">
-            <v>160</v>
-          </cell>
-          <cell r="AX16">
-            <v>2</v>
-          </cell>
         </row>
         <row r="17">
           <cell r="M17">
@@ -3936,15 +3936,6 @@
           </cell>
           <cell r="Z17">
             <v>12</v>
-          </cell>
-          <cell r="AV17">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-          <cell r="AW17">
-            <v>220</v>
-          </cell>
-          <cell r="AX17">
-            <v>2.1</v>
           </cell>
         </row>
         <row r="18">
@@ -3975,15 +3966,6 @@
           <cell r="Z18">
             <v>17</v>
           </cell>
-          <cell r="AV18">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-          <cell r="AW18">
-            <v>240</v>
-          </cell>
-          <cell r="AX18">
-            <v>2.2000000000000002</v>
-          </cell>
         </row>
         <row r="19">
           <cell r="M19">
@@ -4012,15 +3994,6 @@
           </cell>
           <cell r="Z19">
             <v>15</v>
-          </cell>
-          <cell r="AV19">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-          <cell r="AW19">
-            <v>300</v>
-          </cell>
-          <cell r="AX19">
-            <v>2.2999999999999998</v>
           </cell>
         </row>
         <row r="20">
@@ -4051,15 +4024,6 @@
           <cell r="Z20">
             <v>21</v>
           </cell>
-          <cell r="AV20">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-          <cell r="AW20">
-            <v>350</v>
-          </cell>
-          <cell r="AX20">
-            <v>2.4</v>
-          </cell>
         </row>
         <row r="21">
           <cell r="M21">
@@ -4088,15 +4052,6 @@
           </cell>
           <cell r="Z21">
             <v>18</v>
-          </cell>
-          <cell r="AV21">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-          <cell r="AW21">
-            <v>400</v>
-          </cell>
-          <cell r="AX21">
-            <v>2.5</v>
           </cell>
         </row>
         <row r="22">
@@ -4127,15 +4082,6 @@
           <cell r="Z22">
             <v>20</v>
           </cell>
-          <cell r="AV22">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-          <cell r="AW22">
-            <v>440</v>
-          </cell>
-          <cell r="AX22">
-            <v>2.6</v>
-          </cell>
         </row>
         <row r="23">
           <cell r="M23">
@@ -4164,15 +4110,6 @@
           </cell>
           <cell r="Z23">
             <v>28</v>
-          </cell>
-          <cell r="AV23">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-          <cell r="AW23">
-            <v>575</v>
-          </cell>
-          <cell r="AX23">
-            <v>3.2</v>
           </cell>
         </row>
         <row r="24">
@@ -4203,15 +4140,6 @@
           <cell r="Z24">
             <v>25</v>
           </cell>
-          <cell r="AV24">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-          <cell r="AW24">
-            <v>725</v>
-          </cell>
-          <cell r="AX24">
-            <v>3.9</v>
-          </cell>
         </row>
         <row r="25">
           <cell r="M25">
@@ -4240,15 +4168,6 @@
           </cell>
           <cell r="Z25">
             <v>24</v>
-          </cell>
-          <cell r="AV25">
-            <v>5.0000000000000001E-3</v>
-          </cell>
-          <cell r="AW25">
-            <v>900</v>
-          </cell>
-          <cell r="AX25">
-            <v>4.7</v>
           </cell>
         </row>
         <row r="37">
@@ -4704,8 +4623,8 @@
   </sheetPr>
   <dimension ref="D2:O100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O56" sqref="O56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5172,7 +5091,7 @@
       <c r="H24">
         <v>450</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="73" t="s">
         <v>10</v>
       </c>
       <c r="K24" s="73"/>
@@ -6093,7 +6012,7 @@
       <c r="H56">
         <v>450</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="73" t="s">
         <v>10</v>
       </c>
       <c r="K56" s="73"/>
@@ -7391,8 +7310,8 @@
   </sheetPr>
   <dimension ref="B1:U270"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8402,7 +8321,7 @@
       </c>
       <c r="L50" s="10">
         <f>ROUND((DATA_DRAGONS_CONTENT!J5/DATA_DRAGONS_CONTENT!L5)/DATA_DRAGONS_CONTENT!K5,1)</f>
-        <v>0</v>
+        <v>8.4</v>
       </c>
       <c r="N50" s="35">
         <v>0</v>
@@ -8427,11 +8346,11 @@
       </c>
       <c r="L51" s="11">
         <f>ROUND((DATA_DRAGONS_CONTENT!J6/DATA_DRAGONS_CONTENT!L6)/DATA_DRAGONS_CONTENT!K6,1)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N51" s="36">
         <f>L51-L50</f>
-        <v>0</v>
+        <v>2.5999999999999996</v>
       </c>
     </row>
     <row r="52" spans="3:14" x14ac:dyDescent="0.25">
@@ -8453,11 +8372,11 @@
       </c>
       <c r="L52" s="12">
         <f>ROUND((DATA_DRAGONS_CONTENT!J7/DATA_DRAGONS_CONTENT!L7)/DATA_DRAGONS_CONTENT!K7,1)</f>
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="N52" s="36">
         <f t="shared" ref="N52:N59" si="7">L52-L51</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="53" spans="3:14" x14ac:dyDescent="0.25">
@@ -8479,11 +8398,11 @@
       </c>
       <c r="L53" s="12">
         <f>ROUND((DATA_DRAGONS_CONTENT!J8/DATA_DRAGONS_CONTENT!L8)/DATA_DRAGONS_CONTENT!K8,1)</f>
-        <v>0</v>
+        <v>13.7</v>
       </c>
       <c r="N53" s="36">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.1999999999999993</v>
       </c>
     </row>
     <row r="54" spans="3:14" x14ac:dyDescent="0.25">
@@ -8505,11 +8424,11 @@
       </c>
       <c r="L54" s="13">
         <f>ROUND((DATA_DRAGONS_CONTENT!J9/DATA_DRAGONS_CONTENT!L9)/DATA_DRAGONS_CONTENT!K9,1)</f>
-        <v>0</v>
+        <v>15.4</v>
       </c>
       <c r="N54" s="36">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.7000000000000011</v>
       </c>
     </row>
     <row r="55" spans="3:14" x14ac:dyDescent="0.25">
@@ -8531,11 +8450,11 @@
       </c>
       <c r="L55" s="13">
         <f>ROUND((DATA_DRAGONS_CONTENT!J10/DATA_DRAGONS_CONTENT!L10)/DATA_DRAGONS_CONTENT!K10,1)</f>
-        <v>0</v>
+        <v>16.8</v>
       </c>
       <c r="N55" s="36">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.4000000000000004</v>
       </c>
     </row>
     <row r="56" spans="3:14" x14ac:dyDescent="0.25">
@@ -8557,11 +8476,11 @@
       </c>
       <c r="L56" s="14">
         <f>ROUND((DATA_DRAGONS_CONTENT!J11/DATA_DRAGONS_CONTENT!L11)/DATA_DRAGONS_CONTENT!K11,1)</f>
-        <v>0</v>
+        <v>17.8</v>
       </c>
       <c r="N56" s="36">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="3:14" x14ac:dyDescent="0.25">
@@ -8583,11 +8502,11 @@
       </c>
       <c r="L57" s="15">
         <f>ROUND((DATA_DRAGONS_CONTENT!J12/DATA_DRAGONS_CONTENT!L12)/DATA_DRAGONS_CONTENT!K12,1)</f>
-        <v>0</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="N57" s="36">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.0999999999999979</v>
       </c>
     </row>
     <row r="58" spans="3:14" x14ac:dyDescent="0.25">
@@ -8609,11 +8528,11 @@
       </c>
       <c r="L58" s="15">
         <f>ROUND((DATA_DRAGONS_CONTENT!J13/DATA_DRAGONS_CONTENT!L13)/DATA_DRAGONS_CONTENT!K13,1)</f>
-        <v>0</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="N58" s="36">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.70000000000000284</v>
       </c>
     </row>
     <row r="59" spans="3:14" x14ac:dyDescent="0.25">
@@ -8635,11 +8554,11 @@
       </c>
       <c r="L59" s="16">
         <f>ROUND((DATA_DRAGONS_CONTENT!J14/DATA_DRAGONS_CONTENT!L14)/DATA_DRAGONS_CONTENT!K14,1)</f>
-        <v>0</v>
+        <v>20.2</v>
       </c>
       <c r="N59" s="18">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.59999999999999787</v>
       </c>
     </row>
     <row r="60" spans="3:14" x14ac:dyDescent="0.25">
@@ -8776,7 +8695,7 @@
       </c>
       <c r="M66" s="10">
         <f>ROUND(((DATA_DRAGONS_CONTENT!J5*Dragons!L66)/DATA_DRAGONS_CONTENT!L5)/DATA_DRAGONS_CONTENT!K5,1)</f>
-        <v>0</v>
+        <v>16.8</v>
       </c>
       <c r="N66" s="10">
         <f>ROUND(DATA_DRAGONS_CONTENT!N5/DATA_DRAGONS_CONTENT!O5,1)</f>
@@ -8817,7 +8736,7 @@
       </c>
       <c r="M67" s="11">
         <f>ROUND(((DATA_DRAGONS_CONTENT!J6*Dragons!L67)/DATA_DRAGONS_CONTENT!L6)/DATA_DRAGONS_CONTENT!K6,1)</f>
-        <v>0</v>
+        <v>22.1</v>
       </c>
       <c r="N67" s="11">
         <f>ROUND(DATA_DRAGONS_CONTENT!N6/DATA_DRAGONS_CONTENT!O6,1)</f>
@@ -8833,7 +8752,7 @@
       </c>
       <c r="U67" s="36">
         <f t="shared" ref="U67:U75" si="9">M67-M66</f>
-        <v>0</v>
+        <v>5.3000000000000007</v>
       </c>
     </row>
     <row r="68" spans="3:21" x14ac:dyDescent="0.25">
@@ -8859,7 +8778,7 @@
       </c>
       <c r="M68" s="12">
         <f>ROUND(((DATA_DRAGONS_CONTENT!J7*Dragons!L68)/DATA_DRAGONS_CONTENT!L7)/DATA_DRAGONS_CONTENT!K7,1)</f>
-        <v>0</v>
+        <v>21.8</v>
       </c>
       <c r="N68" s="12">
         <f>ROUND(DATA_DRAGONS_CONTENT!N7/DATA_DRAGONS_CONTENT!O7,1)</f>
@@ -8875,7 +8794,7 @@
       </c>
       <c r="U68" s="36">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-0.30000000000000071</v>
       </c>
     </row>
     <row r="69" spans="3:21" x14ac:dyDescent="0.25">
@@ -8901,7 +8820,7 @@
       </c>
       <c r="M69" s="12">
         <f>ROUND(((DATA_DRAGONS_CONTENT!J8*Dragons!L69)/DATA_DRAGONS_CONTENT!L8)/DATA_DRAGONS_CONTENT!K8,1)</f>
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="N69" s="12">
         <f>ROUND(DATA_DRAGONS_CONTENT!N8/DATA_DRAGONS_CONTENT!O8,1)</f>
@@ -8917,7 +8836,7 @@
       </c>
       <c r="U69" s="36">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>5.6999999999999993</v>
       </c>
     </row>
     <row r="70" spans="3:21" x14ac:dyDescent="0.25">
@@ -8943,7 +8862,7 @@
       </c>
       <c r="M70" s="13">
         <f>ROUND(((DATA_DRAGONS_CONTENT!J9*Dragons!L70)/DATA_DRAGONS_CONTENT!L9)/DATA_DRAGONS_CONTENT!K9,1)</f>
-        <v>0</v>
+        <v>27.6</v>
       </c>
       <c r="N70" s="13">
         <f>ROUND(DATA_DRAGONS_CONTENT!N9/DATA_DRAGONS_CONTENT!O9,1)</f>
@@ -8959,7 +8878,7 @@
       </c>
       <c r="U70" s="36">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.10000000000000142</v>
       </c>
     </row>
     <row r="71" spans="3:21" x14ac:dyDescent="0.25">
@@ -8985,7 +8904,7 @@
       </c>
       <c r="M71" s="13">
         <f>ROUND(((DATA_DRAGONS_CONTENT!J10*Dragons!L71)/DATA_DRAGONS_CONTENT!L10)/DATA_DRAGONS_CONTENT!K10,1)</f>
-        <v>0</v>
+        <v>30.3</v>
       </c>
       <c r="N71" s="13">
         <f>ROUND(DATA_DRAGONS_CONTENT!N10/DATA_DRAGONS_CONTENT!O10,1)</f>
@@ -9001,7 +8920,7 @@
       </c>
       <c r="U71" s="36">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>2.6999999999999993</v>
       </c>
     </row>
     <row r="72" spans="3:21" x14ac:dyDescent="0.25">
@@ -9027,7 +8946,7 @@
       </c>
       <c r="M72" s="14">
         <f>ROUND(((DATA_DRAGONS_CONTENT!J11*Dragons!L72)/DATA_DRAGONS_CONTENT!L11)/DATA_DRAGONS_CONTENT!K11,1)</f>
-        <v>0</v>
+        <v>32.1</v>
       </c>
       <c r="N72" s="14">
         <f>ROUND(DATA_DRAGONS_CONTENT!N11/DATA_DRAGONS_CONTENT!O11,1)</f>
@@ -9043,7 +8962,7 @@
       </c>
       <c r="U72" s="36">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1.8000000000000007</v>
       </c>
     </row>
     <row r="73" spans="3:21" x14ac:dyDescent="0.25">
@@ -9069,7 +8988,7 @@
       </c>
       <c r="M73" s="15">
         <f>ROUND(((DATA_DRAGONS_CONTENT!J12*Dragons!L73)/DATA_DRAGONS_CONTENT!L12)/DATA_DRAGONS_CONTENT!K12,1)</f>
-        <v>0</v>
+        <v>30.3</v>
       </c>
       <c r="N73" s="15">
         <f>ROUND(DATA_DRAGONS_CONTENT!N12/DATA_DRAGONS_CONTENT!O12,1)</f>
@@ -9085,7 +9004,7 @@
       </c>
       <c r="U73" s="36">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1.8000000000000007</v>
       </c>
     </row>
     <row r="74" spans="3:21" x14ac:dyDescent="0.25">
@@ -9111,7 +9030,7 @@
       </c>
       <c r="M74" s="15">
         <f>ROUND(((DATA_DRAGONS_CONTENT!J13*Dragons!L74)/DATA_DRAGONS_CONTENT!L13)/DATA_DRAGONS_CONTENT!K13,1)</f>
-        <v>0</v>
+        <v>31.3</v>
       </c>
       <c r="N74" s="15">
         <f>ROUND(DATA_DRAGONS_CONTENT!N13/DATA_DRAGONS_CONTENT!O13,1)</f>
@@ -9127,7 +9046,7 @@
       </c>
       <c r="U74" s="36">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="3:21" x14ac:dyDescent="0.25">
@@ -9153,7 +9072,7 @@
       </c>
       <c r="M75" s="16">
         <f>ROUND(((DATA_DRAGONS_CONTENT!J14*Dragons!L75)/DATA_DRAGONS_CONTENT!L14)/DATA_DRAGONS_CONTENT!K14,1)</f>
-        <v>0</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="N75" s="16">
         <f>ROUND(DATA_DRAGONS_CONTENT!N14/DATA_DRAGONS_CONTENT!O14,1)</f>
@@ -9169,7 +9088,7 @@
       </c>
       <c r="U75" s="18">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.99999999999999645</v>
       </c>
     </row>
     <row r="76" spans="3:21" x14ac:dyDescent="0.25">
@@ -12111,8 +12030,8 @@
   </sheetPr>
   <dimension ref="C3:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12233,7 +12152,7 @@
   <dimension ref="G2:S22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12306,16 +12225,13 @@
         <v>105</v>
       </c>
       <c r="J5" s="10">
-        <f>[1]dragons!$AV$16</f>
-        <v>5.0000000000000001E-3</v>
+        <v>160</v>
       </c>
       <c r="K5" s="10">
-        <f>[1]dragons!$AW$16</f>
-        <v>160</v>
+        <v>2</v>
       </c>
       <c r="L5" s="10">
-        <f>[1]dragons!$AX$16</f>
-        <v>2</v>
+        <v>9.5</v>
       </c>
       <c r="M5" s="10">
         <f>[1]dragons!$W$16</f>
@@ -12359,16 +12275,13 @@
         <v>145</v>
       </c>
       <c r="J6" s="11">
-        <f>[1]dragons!$AV$17</f>
-        <v>5.0000000000000001E-3</v>
+        <v>220</v>
       </c>
       <c r="K6" s="11">
-        <f>[1]dragons!$AW$17</f>
-        <v>220</v>
+        <v>2.1</v>
       </c>
       <c r="L6" s="11">
-        <f>[1]dragons!$AX$17</f>
-        <v>2.1</v>
+        <v>9.5</v>
       </c>
       <c r="M6" s="11">
         <f>[1]dragons!$W$17</f>
@@ -12412,16 +12325,13 @@
         <v>200</v>
       </c>
       <c r="J7" s="12">
-        <f>[1]dragons!$AV$18</f>
-        <v>5.0000000000000001E-3</v>
+        <v>240</v>
       </c>
       <c r="K7" s="12">
-        <f>[1]dragons!$AW$18</f>
-        <v>240</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="L7" s="12">
-        <f>[1]dragons!$AX$18</f>
-        <v>2.2000000000000002</v>
+        <v>9.5</v>
       </c>
       <c r="M7" s="12">
         <f>[1]dragons!$W$18</f>
@@ -12465,16 +12375,13 @@
         <v>220</v>
       </c>
       <c r="J8" s="12">
-        <f>[1]dragons!$AV$19</f>
-        <v>5.0000000000000001E-3</v>
+        <v>300</v>
       </c>
       <c r="K8" s="12">
-        <f>[1]dragons!$AW$19</f>
-        <v>300</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L8" s="12">
-        <f>[1]dragons!$AX$19</f>
-        <v>2.2999999999999998</v>
+        <v>9.5</v>
       </c>
       <c r="M8" s="12">
         <f>[1]dragons!$W$19</f>
@@ -12518,16 +12425,13 @@
         <v>270</v>
       </c>
       <c r="J9" s="13">
-        <f>[1]dragons!$AV$20</f>
-        <v>5.0000000000000001E-3</v>
+        <v>350</v>
       </c>
       <c r="K9" s="13">
-        <f>[1]dragons!$AW$20</f>
-        <v>350</v>
+        <v>2.4</v>
       </c>
       <c r="L9" s="13">
-        <f>[1]dragons!$AX$20</f>
-        <v>2.4</v>
+        <v>9.5</v>
       </c>
       <c r="M9" s="13">
         <f>[1]dragons!$W$20</f>
@@ -12571,16 +12475,13 @@
         <v>310</v>
       </c>
       <c r="J10" s="13">
-        <f>[1]dragons!$AV$21</f>
-        <v>5.0000000000000001E-3</v>
+        <v>400</v>
       </c>
       <c r="K10" s="13">
-        <f>[1]dragons!$AW$21</f>
-        <v>400</v>
+        <v>2.5</v>
       </c>
       <c r="L10" s="13">
-        <f>[1]dragons!$AX$21</f>
-        <v>2.5</v>
+        <v>9.5</v>
       </c>
       <c r="M10" s="13">
         <f>[1]dragons!$W$21</f>
@@ -12624,16 +12525,13 @@
         <v>350</v>
       </c>
       <c r="J11" s="14">
-        <f>[1]dragons!$AV$22</f>
-        <v>5.0000000000000001E-3</v>
+        <v>440</v>
       </c>
       <c r="K11" s="14">
-        <f>[1]dragons!$AW$22</f>
-        <v>440</v>
+        <v>2.6</v>
       </c>
       <c r="L11" s="14">
-        <f>[1]dragons!$AX$22</f>
-        <v>2.6</v>
+        <v>9.5</v>
       </c>
       <c r="M11" s="14">
         <f>[1]dragons!$W$22</f>
@@ -12677,16 +12575,13 @@
         <v>400</v>
       </c>
       <c r="J12" s="15">
-        <f>[1]dragons!$AV$23</f>
-        <v>5.0000000000000001E-3</v>
+        <v>575</v>
       </c>
       <c r="K12" s="15">
-        <f>[1]dragons!$AW$23</f>
-        <v>575</v>
+        <v>3.2</v>
       </c>
       <c r="L12" s="15">
-        <f>[1]dragons!$AX$23</f>
-        <v>3.2</v>
+        <v>9.5</v>
       </c>
       <c r="M12" s="15">
         <f>[1]dragons!$W$23</f>
@@ -12730,16 +12625,13 @@
         <v>445</v>
       </c>
       <c r="J13" s="15">
-        <f>[1]dragons!$AV$24</f>
-        <v>5.0000000000000001E-3</v>
+        <v>725</v>
       </c>
       <c r="K13" s="15">
-        <f>[1]dragons!$AW$24</f>
-        <v>725</v>
+        <v>3.9</v>
       </c>
       <c r="L13" s="15">
-        <f>[1]dragons!$AX$24</f>
-        <v>3.9</v>
+        <v>9.5</v>
       </c>
       <c r="M13" s="15">
         <f>[1]dragons!$W$24</f>
@@ -12783,16 +12675,13 @@
         <v>500</v>
       </c>
       <c r="J14" s="16">
-        <f>[1]dragons!$AV$25</f>
-        <v>5.0000000000000001E-3</v>
+        <v>900</v>
       </c>
       <c r="K14" s="16">
-        <f>[1]dragons!$AW$25</f>
-        <v>900</v>
+        <v>4.7</v>
       </c>
       <c r="L14" s="16">
-        <f>[1]dragons!$AX$25</f>
-        <v>4.7</v>
+        <v>9.5</v>
       </c>
       <c r="M14" s="16">
         <f>[1]dragons!$W$25</f>

</xml_diff>

<commit_message>
Inflammable decorations: set respawn time and duration
Former-commit-id: ee32abb29cb0cc4344ead118ce67a9bd1d57dbbb
</commit_message>
<xml_diff>
--- a/Docs/Progression/progression.xlsx
+++ b/Docs/Progression/progression.xlsx
@@ -5641,8 +5641,8 @@
   </sheetPr>
   <dimension ref="D2:O103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>